<commit_message>
Se implemento analisis con sonarQube
Se añadieron mas sujetos de prueba, junto con sus analisis.
</commit_message>
<xml_diff>
--- a/Carpeta de Estudio/Historial de Repositorios.xlsx
+++ b/Carpeta de Estudio/Historial de Repositorios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jorge\OneDrive\Documentos\GitHub\MIC-Evolucion_patrones_de_diseno\Carpeta de Estudio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC567F12-8A91-4BB6-8246-BFA0FCAC7F59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6839C7DF-6688-4560-884B-E94CD76CF9AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{EE91BF2F-F0DA-4949-BD11-E6893A9471D6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="76">
   <si>
     <t>Usuario</t>
   </si>
@@ -62,9 +62,6 @@
     <t>E01</t>
   </si>
   <si>
-    <t>LuisJs</t>
-  </si>
-  <si>
     <t>E02</t>
   </si>
   <si>
@@ -174,6 +171,99 @@
   </si>
   <si>
     <t>LeoParra03</t>
+  </si>
+  <si>
+    <t>ConcesionariaDeAutos</t>
+  </si>
+  <si>
+    <t>jekins</t>
+  </si>
+  <si>
+    <t>amadoran</t>
+  </si>
+  <si>
+    <t>E12</t>
+  </si>
+  <si>
+    <t>Calculadora</t>
+  </si>
+  <si>
+    <t>kgjara</t>
+  </si>
+  <si>
+    <t>E13</t>
+  </si>
+  <si>
+    <t>EmojiBuilder</t>
+  </si>
+  <si>
+    <t>tresEnRaya</t>
+  </si>
+  <si>
+    <t>Luisenjs</t>
+  </si>
+  <si>
+    <t>julioguerrero131</t>
+  </si>
+  <si>
+    <t>E14</t>
+  </si>
+  <si>
+    <t>pagina_web-food_store-html-css-js</t>
+  </si>
+  <si>
+    <t>MichaelJimenezC</t>
+  </si>
+  <si>
+    <t>E15</t>
+  </si>
+  <si>
+    <t>Tetris</t>
+  </si>
+  <si>
+    <t>algo</t>
+  </si>
+  <si>
+    <t>leoancab</t>
+  </si>
+  <si>
+    <t>E16</t>
+  </si>
+  <si>
+    <t>welleats</t>
+  </si>
+  <si>
+    <t>Botsongs</t>
+  </si>
+  <si>
+    <t>Nasdj21</t>
+  </si>
+  <si>
+    <t>E17</t>
+  </si>
+  <si>
+    <t>Proyecto_EDD </t>
+  </si>
+  <si>
+    <t>ProyectoPooBacan</t>
+  </si>
+  <si>
+    <t>RecorridoHeap</t>
+  </si>
+  <si>
+    <t>PokeAPI_DAWM</t>
+  </si>
+  <si>
+    <t>E18</t>
+  </si>
+  <si>
+    <t>DavidlunaT</t>
+  </si>
+  <si>
+    <t>G3_Estructura-de-datos1_Luna_Jimenez_Yagual</t>
+  </si>
+  <si>
+    <t>EDD_2</t>
   </si>
 </sst>
 </file>
@@ -225,10 +315,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -564,17 +657,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A5EA97E-D124-4C52-BAED-29F745ABDAB8}">
-  <dimension ref="C4:F15"/>
+  <dimension ref="C4:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="27.5703125" customWidth="1"/>
     <col min="4" max="4" width="18.42578125" customWidth="1"/>
-    <col min="5" max="5" width="36.85546875" customWidth="1"/>
+    <col min="5" max="5" width="44.85546875" customWidth="1"/>
     <col min="6" max="6" width="29.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -608,136 +701,240 @@
     </row>
     <row r="6" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D6" t="s">
         <v>8</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="F6" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="7" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" t="s">
         <v>12</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>13</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>14</v>
-      </c>
-      <c r="F7" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="8" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" t="s">
         <v>16</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="F8" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="9" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" t="s">
         <v>20</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="F9" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="10" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" t="s">
         <v>25</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" t="s">
         <v>26</v>
-      </c>
-      <c r="E10" t="s">
-        <v>24</v>
-      </c>
-      <c r="F10" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="11" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" t="s">
         <v>28</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="F11" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="12" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" t="s">
         <v>32</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="F12" t="s">
         <v>34</v>
-      </c>
-      <c r="F12" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="13" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" t="s">
         <v>36</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>37</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>38</v>
-      </c>
-      <c r="F13" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="14" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" t="s">
+        <v>39</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D14" t="s">
-        <v>40</v>
-      </c>
-      <c r="E14" s="2" t="s">
+      <c r="F14" t="s">
         <v>42</v>
-      </c>
-      <c r="F14" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="15" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
+        <v>44</v>
+      </c>
+      <c r="D15" t="s">
+        <v>43</v>
+      </c>
+      <c r="E15" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D15" t="s">
-        <v>44</v>
+      <c r="F15" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>47</v>
+      </c>
+      <c r="D16" t="s">
+        <v>48</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F16" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>50</v>
+      </c>
+      <c r="D17" t="s">
+        <v>51</v>
+      </c>
+      <c r="E17" t="s">
+        <v>52</v>
+      </c>
+      <c r="F17" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>55</v>
+      </c>
+      <c r="D18" t="s">
+        <v>56</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="19" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>58</v>
+      </c>
+      <c r="D19" t="s">
+        <v>59</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F19" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="20" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>62</v>
+      </c>
+      <c r="D20" t="s">
+        <v>63</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F20" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="21" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>66</v>
+      </c>
+      <c r="D21" t="s">
+        <v>67</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="22" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>73</v>
+      </c>
+      <c r="D22" t="s">
+        <v>72</v>
+      </c>
+      <c r="E22" t="s">
+        <v>74</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -753,8 +950,17 @@
     <hyperlink ref="F11" r:id="rId9" display="https://github.com/jcvivas/Java-OOP-Shop" xr:uid="{6B99E77D-D480-4453-8917-FD8A463EFA78}"/>
     <hyperlink ref="E12" r:id="rId10" display="https://github.com/anarjumb/Proyecto1P" xr:uid="{456E6A08-6B2F-4934-8C9A-C245F973562E}"/>
     <hyperlink ref="E14" r:id="rId11" display="https://github.com/RobertoPatino1/ProyectoMatematicasDiscretas" xr:uid="{A66EB3B4-04AF-480F-BE82-E5B96EF2B38B}"/>
+    <hyperlink ref="E15" r:id="rId12" display="https://github.com/LeoParra03/ConcesionariaDeAutos" xr:uid="{EB71A70A-5B2E-482B-8E71-CEAAF986DE68}"/>
+    <hyperlink ref="F18" r:id="rId13" display="https://github.com/julioguerrero131/pagina_web-food_store-html-css-js" xr:uid="{10143001-85FA-4F69-A5DA-EE944303774C}"/>
+    <hyperlink ref="E19" r:id="rId14" display="https://github.com/MichaelJimenezC/Tetris" xr:uid="{69D8F13D-7B6B-410E-B99A-FD598AAFD301}"/>
+    <hyperlink ref="E20" r:id="rId15" display="https://github.com/leoancab/welleats" xr:uid="{8E8E1EA7-B656-4CE3-8BF4-43066236C00E}"/>
+    <hyperlink ref="F21" r:id="rId16" display="https://github.com/nasdj21/Proyecto_EDD" xr:uid="{DFB9BB5C-03CA-4453-9ED8-45C5D18C1C7F}"/>
+    <hyperlink ref="E21" r:id="rId17" display="https://github.com/nasdj21/ProyectoPooBacan" xr:uid="{2E089D91-C88F-4B74-8563-A75CF6EFAD68}"/>
+    <hyperlink ref="E16" r:id="rId18" display="https://github.com/amadoran/RecorridoHeap" xr:uid="{C522E359-CFF9-4F8F-8674-5F18EA16CAA8}"/>
+    <hyperlink ref="E18" r:id="rId19" display="https://github.com/julioguerrero131/PokeAPI_DAWM" xr:uid="{5017E2FF-4D5B-4A22-87F4-9CE3935B247F}"/>
+    <hyperlink ref="F22" r:id="rId20" display="https://github.com/DavidlunaT/EDD_2" xr:uid="{3953976A-6CAD-45D3-AE16-FAFC7705883D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId12"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId21"/>
 </worksheet>
 </file>
</xml_diff>